<commit_message>
fixing of excel file, labels of barplots and text for how variables are coded
</commit_message>
<xml_diff>
--- a/wikishootings_final.xlsx
+++ b/wikishootings_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hre\Documents\Uni_Mannheim\FSS_2020\Research_Methods_Fundamentals_of_Computing_and_Data_Display\Paper\Term-Paper-Fundamentals\Fundamentals---Term-Paper-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6125E07A-254F-48F9-9DBD-6D8691ABB040}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98352A0A-2A19-4BA7-B4A6-52142D887657}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1977,7 +1977,7 @@
   <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2052,13 +2052,13 @@
         <v>9</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2090,13 +2090,13 @@
         <v>8</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2128,13 +2128,13 @@
         <v>8</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2166,13 +2166,13 @@
         <v>12</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2204,13 +2204,13 @@
         <v>15</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2242,13 +2242,13 @@
         <v>6</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2280,13 +2280,13 @@
         <v>8</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -2318,13 +2318,13 @@
         <v>9</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2356,13 +2356,13 @@
         <v>7</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -2394,13 +2394,13 @@
         <v>11</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2432,13 +2432,13 @@
         <v>10</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2470,13 +2470,13 @@
         <v>50</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2508,13 +2508,13 @@
         <v>8</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2546,13 +2546,13 @@
         <v>15</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2584,13 +2584,13 @@
         <v>10</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2660,13 +2660,13 @@
         <v>8</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2698,13 +2698,13 @@
         <v>27</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2742,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2774,13 +2774,13 @@
         <v>13</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2812,13 +2812,13 @@
         <v>17</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2850,13 +2850,13 @@
         <v>11</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2888,13 +2888,13 @@
         <v>18</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2926,13 +2926,13 @@
         <v>6</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2964,13 +2964,13 @@
         <v>13</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -3002,13 +3002,13 @@
         <v>47</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -3040,13 +3040,13 @@
         <v>9</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -3078,13 +3078,13 @@
         <v>6</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
         <v>1</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -3154,13 +3154,13 @@
         <v>11</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <v>1</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -3192,13 +3192,13 @@
         <v>21</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>1</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -3230,13 +3230,13 @@
         <v>10</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33">
         <v>1</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -3268,13 +3268,13 @@
         <v>9</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>1</v>
       </c>
       <c r="L34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -3306,13 +3306,13 @@
         <v>12</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -3344,13 +3344,13 @@
         <v>9</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>1</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -3382,13 +3382,13 @@
         <v>5</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37">
         <v>1</v>
       </c>
       <c r="L37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -3420,13 +3420,13 @@
         <v>6</v>
       </c>
       <c r="J38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38">
         <v>1</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -3458,13 +3458,13 @@
         <v>10</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39">
         <v>1</v>
       </c>
       <c r="L39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -3496,13 +3496,13 @@
         <v>7</v>
       </c>
       <c r="J40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40">
         <v>1</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -3534,13 +3534,13 @@
         <v>82</v>
       </c>
       <c r="J41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41">
         <v>1</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -3572,13 +3572,13 @@
         <v>11</v>
       </c>
       <c r="J42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="L42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -3610,13 +3610,13 @@
         <v>7</v>
       </c>
       <c r="J43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -3648,13 +3648,13 @@
         <v>11</v>
       </c>
       <c r="J44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44">
         <v>1</v>
       </c>
       <c r="L44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -3686,13 +3686,13 @@
         <v>9</v>
       </c>
       <c r="J45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="L45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -3724,13 +3724,13 @@
         <v>8</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46">
         <v>1</v>
       </c>
       <c r="L46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -3768,7 +3768,7 @@
         <v>1</v>
       </c>
       <c r="L47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -3800,13 +3800,13 @@
         <v>30</v>
       </c>
       <c r="J48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48">
         <v>1</v>
       </c>
       <c r="L48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -3838,13 +3838,13 @@
         <v>7</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49">
         <v>1</v>
       </c>
       <c r="L49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -3876,13 +3876,13 @@
         <v>5</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
       <c r="L50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -3914,13 +3914,13 @@
         <v>11</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51">
         <v>1</v>
       </c>
       <c r="L51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -3952,13 +3952,13 @@
         <v>7</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52">
         <v>0</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3990,13 +3990,13 @@
         <v>7</v>
       </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <v>1</v>
       </c>
       <c r="L53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -4028,13 +4028,13 @@
         <v>21</v>
       </c>
       <c r="J54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54">
         <v>1</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -4072,7 +4072,7 @@
         <v>1</v>
       </c>
       <c r="L55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -4104,13 +4104,13 @@
         <v>18</v>
       </c>
       <c r="J56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56">
         <v>0</v>
       </c>
       <c r="L56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -4142,13 +4142,13 @@
         <v>20</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K57">
         <v>0</v>
       </c>
       <c r="L57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -4180,13 +4180,13 @@
         <v>7</v>
       </c>
       <c r="J58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K58">
         <v>1</v>
       </c>
       <c r="L58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -4218,13 +4218,13 @@
         <v>6</v>
       </c>
       <c r="J59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59">
         <v>1</v>
       </c>
       <c r="L59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -4256,13 +4256,13 @@
         <v>4</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K60">
         <v>1</v>
       </c>
       <c r="L60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -4294,13 +4294,13 @@
         <v>7</v>
       </c>
       <c r="J61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K61">
         <v>1</v>
       </c>
       <c r="L61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -4332,13 +4332,13 @@
         <v>9</v>
       </c>
       <c r="J62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62">
         <v>0</v>
       </c>
       <c r="L62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
@@ -4376,7 +4376,7 @@
         <v>0</v>
       </c>
       <c r="L63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -4408,13 +4408,13 @@
         <v>10</v>
       </c>
       <c r="J64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K64">
         <v>1</v>
       </c>
       <c r="L64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -4446,13 +4446,13 @@
         <v>8</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
       <c r="L65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -4484,13 +4484,13 @@
         <v>12</v>
       </c>
       <c r="J66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K66">
         <v>1</v>
       </c>
       <c r="L66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -4522,13 +4522,13 @@
         <v>8</v>
       </c>
       <c r="J67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K67">
         <v>1</v>
       </c>
       <c r="L67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -4560,13 +4560,13 @@
         <v>4</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
       <c r="L68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -4598,13 +4598,13 @@
         <v>18</v>
       </c>
       <c r="J69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K69">
         <v>0</v>
       </c>
       <c r="L69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -4636,13 +4636,13 @@
         <v>5</v>
       </c>
       <c r="J70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K70">
         <v>1</v>
       </c>
       <c r="L70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -4674,13 +4674,13 @@
         <v>12</v>
       </c>
       <c r="J71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71">
         <v>1</v>
       </c>
       <c r="L71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -4712,13 +4712,13 @@
         <v>38</v>
       </c>
       <c r="J72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72">
         <v>0</v>
       </c>
       <c r="L72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -4750,13 +4750,13 @@
         <v>8</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73">
         <v>1</v>
       </c>
       <c r="L73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -4788,13 +4788,13 @@
         <v>18</v>
       </c>
       <c r="J74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K74">
         <v>1</v>
       </c>
       <c r="L74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -4832,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="L75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -4864,13 +4864,13 @@
         <v>103</v>
       </c>
       <c r="J76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K76">
         <v>1</v>
       </c>
       <c r="L76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -4902,13 +4902,13 @@
         <v>17</v>
       </c>
       <c r="J77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K77">
         <v>1</v>
       </c>
       <c r="L77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -4940,13 +4940,13 @@
         <v>5</v>
       </c>
       <c r="J78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K78">
         <v>1</v>
       </c>
       <c r="L78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -4978,13 +4978,13 @@
         <v>7</v>
       </c>
       <c r="J79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K79">
         <v>0</v>
       </c>
       <c r="L79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -5016,13 +5016,13 @@
         <v>4</v>
       </c>
       <c r="J80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K80">
         <v>1</v>
       </c>
       <c r="L80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -5054,13 +5054,13 @@
         <v>6</v>
       </c>
       <c r="J81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K81">
         <v>0</v>
       </c>
       <c r="L81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -5092,13 +5092,13 @@
         <v>5</v>
       </c>
       <c r="J82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K82">
         <v>1</v>
       </c>
       <c r="L82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -5130,13 +5130,13 @@
         <v>5</v>
       </c>
       <c r="J83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K83">
         <v>1</v>
       </c>
       <c r="L83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -5168,13 +5168,13 @@
         <v>11</v>
       </c>
       <c r="J84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K84">
         <v>1</v>
       </c>
       <c r="L84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
@@ -5206,13 +5206,13 @@
         <v>5</v>
       </c>
       <c r="J85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K85">
         <v>1</v>
       </c>
       <c r="L85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
@@ -5244,13 +5244,13 @@
         <v>18</v>
       </c>
       <c r="J86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K86">
         <v>0</v>
       </c>
       <c r="L86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
@@ -5282,13 +5282,13 @@
         <v>4</v>
       </c>
       <c r="J87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K87">
         <v>0</v>
       </c>
       <c r="L87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
@@ -5320,13 +5320,13 @@
         <v>4</v>
       </c>
       <c r="J88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K88">
         <v>1</v>
       </c>
       <c r="L88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
@@ -5358,13 +5358,13 @@
         <v>9</v>
       </c>
       <c r="J89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K89">
         <v>0</v>
       </c>
       <c r="L89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
@@ -5396,13 +5396,13 @@
         <v>6</v>
       </c>
       <c r="J90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K90">
         <v>1</v>
       </c>
       <c r="L90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
@@ -5434,13 +5434,13 @@
         <v>5</v>
       </c>
       <c r="J91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K91">
         <v>1</v>
       </c>
       <c r="L91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
@@ -5472,13 +5472,13 @@
         <v>4</v>
       </c>
       <c r="J92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K92">
         <v>0</v>
       </c>
       <c r="L92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
@@ -5510,13 +5510,13 @@
         <v>9</v>
       </c>
       <c r="J93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K93">
         <v>1</v>
       </c>
       <c r="L93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
@@ -5548,13 +5548,13 @@
         <v>7</v>
       </c>
       <c r="J94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K94">
         <v>1</v>
       </c>
       <c r="L94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
@@ -5586,13 +5586,13 @@
         <v>8</v>
       </c>
       <c r="J95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K95">
         <v>0</v>
       </c>
       <c r="L95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
@@ -5630,7 +5630,7 @@
         <v>1</v>
       </c>
       <c r="L96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
@@ -5662,13 +5662,13 @@
         <v>6</v>
       </c>
       <c r="J97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K97">
         <v>0</v>
       </c>
       <c r="L97">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
@@ -5700,13 +5700,13 @@
         <v>10</v>
       </c>
       <c r="J98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K98">
         <v>1</v>
       </c>
       <c r="L98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
@@ -5738,13 +5738,13 @@
         <v>9</v>
       </c>
       <c r="J99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K99">
         <v>1</v>
       </c>
       <c r="L99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
@@ -5776,13 +5776,13 @@
         <v>481</v>
       </c>
       <c r="J100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K100">
         <v>1</v>
       </c>
       <c r="L100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
@@ -5814,13 +5814,13 @@
         <v>47</v>
       </c>
       <c r="J101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K101">
         <v>1</v>
       </c>
       <c r="L101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
@@ -5852,13 +5852,13 @@
         <v>18</v>
       </c>
       <c r="J102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K102">
         <v>0</v>
       </c>
       <c r="L102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
@@ -5890,13 +5890,13 @@
         <v>3</v>
       </c>
       <c r="J103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K103">
         <v>0</v>
       </c>
       <c r="L103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
@@ -5928,13 +5928,13 @@
         <v>8</v>
       </c>
       <c r="J104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K104">
         <v>1</v>
       </c>
       <c r="L104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
@@ -5966,13 +5966,13 @@
         <v>18</v>
       </c>
       <c r="J105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K105">
         <v>1</v>
       </c>
       <c r="L105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
@@ -6004,13 +6004,13 @@
         <v>6</v>
       </c>
       <c r="J106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K106">
         <v>0</v>
       </c>
       <c r="L106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
@@ -6042,13 +6042,13 @@
         <v>34</v>
       </c>
       <c r="J107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K107">
         <v>1</v>
       </c>
       <c r="L107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
@@ -6080,13 +6080,13 @@
         <v>5</v>
       </c>
       <c r="J108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K108">
         <v>1</v>
       </c>
       <c r="L108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
@@ -6118,13 +6118,13 @@
         <v>5</v>
       </c>
       <c r="J109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K109">
         <v>1</v>
       </c>
       <c r="L109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
@@ -6156,13 +6156,13 @@
         <v>6</v>
       </c>
       <c r="J110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K110">
         <v>1</v>
       </c>
       <c r="L110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.3">
@@ -6194,13 +6194,13 @@
         <v>24</v>
       </c>
       <c r="J111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K111">
         <v>1</v>
       </c>
       <c r="L111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
@@ -6232,13 +6232,13 @@
         <v>23</v>
       </c>
       <c r="J112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K112">
         <v>0</v>
       </c>
       <c r="L112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.3">
@@ -6270,13 +6270,13 @@
         <v>7</v>
       </c>
       <c r="J113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K113">
         <v>1</v>
       </c>
       <c r="L113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.3">
@@ -6308,13 +6308,13 @@
         <v>14</v>
       </c>
       <c r="J114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K114">
         <v>1</v>
       </c>
       <c r="L114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.3">
@@ -6346,13 +6346,13 @@
         <v>6</v>
       </c>
       <c r="J115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K115">
         <v>0</v>
       </c>
       <c r="L115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.3">
@@ -6384,13 +6384,13 @@
         <v>7</v>
       </c>
       <c r="J116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K116">
         <v>1</v>
       </c>
       <c r="L116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.3">
@@ -6422,13 +6422,13 @@
         <v>12</v>
       </c>
       <c r="J117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K117">
         <v>1</v>
       </c>
       <c r="L117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.3">
@@ -6460,13 +6460,13 @@
         <v>18</v>
       </c>
       <c r="J118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K118">
         <v>1</v>
       </c>
       <c r="L118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.3">
@@ -6498,13 +6498,13 @@
         <v>8</v>
       </c>
       <c r="J119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K119">
         <v>0</v>
       </c>
       <c r="L119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
@@ -6536,13 +6536,13 @@
         <v>25</v>
       </c>
       <c r="J120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K120">
         <v>1</v>
       </c>
       <c r="L120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
@@ -6574,13 +6574,13 @@
         <v>5</v>
       </c>
       <c r="J121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K121">
         <v>0</v>
       </c>
       <c r="L121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
@@ -6612,13 +6612,13 @@
         <v>4</v>
       </c>
       <c r="J122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K122">
         <v>1</v>
       </c>
       <c r="L122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
@@ -6650,13 +6650,13 @@
         <v>5</v>
       </c>
       <c r="J123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K123">
         <v>0</v>
       </c>
       <c r="L123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
@@ -6688,13 +6688,13 @@
         <v>5</v>
       </c>
       <c r="J124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K124">
         <v>1</v>
       </c>
       <c r="L124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
@@ -6726,13 +6726,13 @@
         <v>12</v>
       </c>
       <c r="J125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K125">
         <v>1</v>
       </c>
       <c r="L125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
@@ -6764,13 +6764,13 @@
         <v>4</v>
       </c>
       <c r="J126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K126">
         <v>1</v>
       </c>
       <c r="L126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
@@ -6802,13 +6802,13 @@
         <v>6</v>
       </c>
       <c r="J127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K127">
         <v>1</v>
       </c>
       <c r="L127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
@@ -6840,13 +6840,13 @@
         <v>9</v>
       </c>
       <c r="J128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K128">
         <v>1</v>
       </c>
       <c r="L128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.3">
@@ -6878,13 +6878,13 @@
         <v>18</v>
       </c>
       <c r="J129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K129">
         <v>1</v>
       </c>
       <c r="L129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.3">
@@ -6916,13 +6916,13 @@
         <v>19</v>
       </c>
       <c r="J130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K130">
         <v>1</v>
       </c>
       <c r="L130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.3">
@@ -6954,13 +6954,13 @@
         <v>46</v>
       </c>
       <c r="J131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K131">
         <v>1</v>
       </c>
       <c r="L131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
@@ -6992,13 +6992,13 @@
         <v>37</v>
       </c>
       <c r="J132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K132">
         <v>0</v>
       </c>
       <c r="L132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
@@ -7030,13 +7030,13 @@
         <v>33</v>
       </c>
       <c r="J133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K133">
         <v>1</v>
       </c>
       <c r="L133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
@@ -7068,13 +7068,13 @@
         <v>9</v>
       </c>
       <c r="J134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K134">
         <v>1</v>
       </c>
       <c r="L134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
@@ -7106,13 +7106,13 @@
         <v>6</v>
       </c>
       <c r="J135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K135">
         <v>1</v>
       </c>
       <c r="L135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.3">
@@ -7144,13 +7144,13 @@
         <v>10</v>
       </c>
       <c r="J136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K136">
         <v>1</v>
       </c>
       <c r="L136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
@@ -7182,13 +7182,13 @@
         <v>5</v>
       </c>
       <c r="J137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K137">
         <v>1</v>
       </c>
       <c r="L137">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.3">
@@ -7220,13 +7220,13 @@
         <v>12</v>
       </c>
       <c r="J138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K138">
         <v>1</v>
       </c>
       <c r="L138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
@@ -7258,13 +7258,13 @@
         <v>9</v>
       </c>
       <c r="J139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K139">
         <v>1</v>
       </c>
       <c r="L139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.3">
@@ -7296,13 +7296,13 @@
         <v>5</v>
       </c>
       <c r="J140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K140">
         <v>1</v>
       </c>
       <c r="L140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
@@ -7334,13 +7334,13 @@
         <v>6</v>
       </c>
       <c r="J141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K141">
         <v>0</v>
       </c>
       <c r="L141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>